<commit_message>
New Design and added tabs (irrigation, profiles)
</commit_message>
<xml_diff>
--- a/SUEWS_db.xlsx
+++ b/SUEWS_db.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" tabRatio="1000" firstSheet="5" activeTab="16"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" tabRatio="1000" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Lod1_Types" sheetId="1" r:id="rId1"/>
@@ -1506,9 +1506,6 @@
     <t>NonVeg10</t>
   </si>
   <si>
-    <t>Copacabanana</t>
-  </si>
-  <si>
     <t>NonVeg11</t>
   </si>
   <si>
@@ -2077,6 +2074,9 @@
   </si>
   <si>
     <t>Gränna</t>
+  </si>
+  <si>
+    <t>Copacabana</t>
   </si>
 </sst>
 </file>
@@ -2566,7 +2566,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -2625,7 +2625,7 @@
         <v>14</v>
       </c>
       <c r="G2" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="H2" t="s">
         <v>15</v>
@@ -2643,10 +2643,10 @@
         <v>19</v>
       </c>
       <c r="M2" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="N2" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -2669,7 +2669,7 @@
         <v>14</v>
       </c>
       <c r="G3" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="H3" t="s">
         <v>15</v>
@@ -2687,10 +2687,10 @@
         <v>23</v>
       </c>
       <c r="M3" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="N3" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -2713,7 +2713,7 @@
         <v>14</v>
       </c>
       <c r="G4" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="H4" t="s">
         <v>15</v>
@@ -2731,10 +2731,10 @@
         <v>19</v>
       </c>
       <c r="M4" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="N4" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -2745,19 +2745,19 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
+        <v>654</v>
+      </c>
+      <c r="D5" t="s">
+        <v>656</v>
+      </c>
+      <c r="E5" t="s">
         <v>655</v>
-      </c>
-      <c r="D5" t="s">
-        <v>657</v>
-      </c>
-      <c r="E5" t="s">
-        <v>656</v>
       </c>
       <c r="F5" t="s">
         <v>14</v>
       </c>
       <c r="G5" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="H5" t="s">
         <v>15</v>
@@ -2775,10 +2775,10 @@
         <v>23</v>
       </c>
       <c r="M5" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="N5" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -2798,7 +2798,7 @@
         <v>14</v>
       </c>
       <c r="G6" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="H6" t="s">
         <v>15</v>
@@ -2816,10 +2816,10 @@
         <v>19</v>
       </c>
       <c r="M6" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="N6" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -2854,10 +2854,10 @@
         <v>19</v>
       </c>
       <c r="M7" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="N7" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -2877,7 +2877,7 @@
         <v>14</v>
       </c>
       <c r="G8" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="H8" t="s">
         <v>36</v>
@@ -2895,10 +2895,10 @@
         <v>23</v>
       </c>
       <c r="M8" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="N8" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -2933,10 +2933,10 @@
         <v>19</v>
       </c>
       <c r="M9" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="N9" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -2971,10 +2971,10 @@
         <v>23</v>
       </c>
       <c r="M10" t="s">
+        <v>490</v>
+      </c>
+      <c r="N10" t="s">
         <v>491</v>
-      </c>
-      <c r="N10" t="s">
-        <v>492</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -2994,7 +2994,7 @@
         <v>14</v>
       </c>
       <c r="G11" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="H11" t="s">
         <v>36</v>
@@ -3012,10 +3012,10 @@
         <v>19</v>
       </c>
       <c r="M11" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="N11" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -3050,10 +3050,10 @@
         <v>23</v>
       </c>
       <c r="M12" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="N12" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -3073,7 +3073,7 @@
         <v>14</v>
       </c>
       <c r="G13" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="H13" t="s">
         <v>36</v>
@@ -3091,10 +3091,10 @@
         <v>19</v>
       </c>
       <c r="M13" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="N13" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -3129,10 +3129,10 @@
         <v>23</v>
       </c>
       <c r="M14" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="N14" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -3167,10 +3167,10 @@
         <v>19</v>
       </c>
       <c r="M15" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="N15" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -3205,10 +3205,10 @@
         <v>23</v>
       </c>
       <c r="M16" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="N16" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
@@ -3249,10 +3249,10 @@
         <v>19</v>
       </c>
       <c r="M17" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="N17" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
@@ -3266,16 +3266,16 @@
         <v>49</v>
       </c>
       <c r="D18" t="s">
+        <v>494</v>
+      </c>
+      <c r="E18" t="s">
         <v>495</v>
-      </c>
-      <c r="E18" t="s">
-        <v>496</v>
       </c>
       <c r="F18" t="s">
         <v>14</v>
       </c>
       <c r="G18" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="H18" t="s">
         <v>51</v>
@@ -3293,10 +3293,10 @@
         <v>22</v>
       </c>
       <c r="M18" t="s">
+        <v>490</v>
+      </c>
+      <c r="N18" t="s">
         <v>491</v>
-      </c>
-      <c r="N18" t="s">
-        <v>492</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
@@ -3319,7 +3319,7 @@
         <v>14</v>
       </c>
       <c r="G19" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="H19" t="s">
         <v>54</v>
@@ -3337,10 +3337,10 @@
         <v>22</v>
       </c>
       <c r="M19" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="N19" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
   </sheetData>
@@ -3377,7 +3377,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>392</v>
@@ -3400,7 +3400,7 @@
         <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="E2" t="s">
         <v>395</v>
@@ -3426,10 +3426,10 @@
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E3" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="F3">
         <v>0.15</v>
@@ -3452,7 +3452,7 @@
         <v>371</v>
       </c>
       <c r="D4" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E4" t="s">
         <v>71</v>
@@ -3478,10 +3478,10 @@
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E5" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="F5">
         <v>0.12</v>
@@ -3504,10 +3504,10 @@
         <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="E6" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="F6">
         <v>0.15</v>
@@ -3530,7 +3530,7 @@
         <v>371</v>
       </c>
       <c r="D7" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="E7" t="s">
         <v>458</v>
@@ -3556,10 +3556,10 @@
         <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="E8" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="F8">
         <v>0.1</v>
@@ -3582,7 +3582,7 @@
         <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="E9" t="s">
         <v>486</v>
@@ -3608,7 +3608,7 @@
         <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="E10" t="s">
         <v>487</v>
@@ -3634,10 +3634,10 @@
         <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E11" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="F11">
         <v>0.1</v>
@@ -3660,10 +3660,10 @@
         <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E12" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="F12">
         <v>0.16</v>
@@ -3686,10 +3686,10 @@
         <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="E13" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="F13">
         <v>0.19</v>
@@ -3703,7 +3703,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B14" t="s">
         <v>367</v>
@@ -3712,10 +3712,10 @@
         <v>482</v>
       </c>
       <c r="D14" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E14" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="F14">
         <v>0.1</v>
@@ -3729,7 +3729,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B15" t="s">
         <v>367</v>
@@ -3738,10 +3738,10 @@
         <v>482</v>
       </c>
       <c r="D15" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="E15" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F15">
         <v>0.1</v>
@@ -3755,7 +3755,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="B16" t="s">
         <v>367</v>
@@ -3764,7 +3764,7 @@
         <v>482</v>
       </c>
       <c r="D16" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="E16" t="s">
         <v>487</v>
@@ -3781,7 +3781,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="B17" t="s">
         <v>363</v>
@@ -3790,10 +3790,10 @@
         <v>6</v>
       </c>
       <c r="D17" t="s">
+        <v>675</v>
+      </c>
+      <c r="E17" t="s">
         <v>676</v>
-      </c>
-      <c r="E17" t="s">
-        <v>677</v>
       </c>
       <c r="F17">
         <v>0.1</v>
@@ -3834,19 +3834,19 @@
         <v>2</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>382</v>
       </c>
       <c r="G1" s="6" t="s">
+        <v>589</v>
+      </c>
+      <c r="H1" s="6" t="s">
         <v>590</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>591</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>592</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>361</v>
@@ -3854,7 +3854,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B2" t="s">
         <v>367</v>
@@ -3863,7 +3863,7 @@
         <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="E2" t="s">
         <v>395</v>
@@ -3886,7 +3886,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B3" t="s">
         <v>367</v>
@@ -3895,10 +3895,10 @@
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E3" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="F3" t="s">
         <v>387</v>
@@ -3918,7 +3918,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B4" t="s">
         <v>367</v>
@@ -3927,7 +3927,7 @@
         <v>371</v>
       </c>
       <c r="D4" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E4" t="s">
         <v>71</v>
@@ -3950,7 +3950,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="B5" t="s">
         <v>367</v>
@@ -3959,13 +3959,13 @@
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E5" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="F5" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="G5">
         <v>7.0000000000000007E-2</v>
@@ -3982,7 +3982,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B6" t="s">
         <v>367</v>
@@ -3991,10 +3991,10 @@
         <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="E6" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="F6" t="s">
         <v>387</v>
@@ -4014,7 +4014,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="B7" t="s">
         <v>367</v>
@@ -4023,7 +4023,7 @@
         <v>371</v>
       </c>
       <c r="D7" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="E7" t="s">
         <v>458</v>
@@ -4046,7 +4046,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B8" t="s">
         <v>363</v>
@@ -4055,10 +4055,10 @@
         <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="E8" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="F8" t="s">
         <v>390</v>
@@ -4078,7 +4078,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B9" t="s">
         <v>363</v>
@@ -4087,13 +4087,13 @@
         <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="E9" t="s">
         <v>486</v>
       </c>
       <c r="F9" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="G9">
         <v>4.2000000000000003E-2</v>
@@ -4110,7 +4110,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B10" t="s">
         <v>363</v>
@@ -4119,7 +4119,7 @@
         <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="E10" t="s">
         <v>487</v>
@@ -4142,7 +4142,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B11" t="s">
         <v>363</v>
@@ -4151,10 +4151,10 @@
         <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E11" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="F11" t="s">
         <v>387</v>
@@ -4174,7 +4174,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B12" t="s">
         <v>363</v>
@@ -4183,10 +4183,10 @@
         <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E12" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="F12" t="s">
         <v>390</v>
@@ -4206,7 +4206,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B13" t="s">
         <v>363</v>
@@ -4215,13 +4215,13 @@
         <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="E13" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="F13" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="G13">
         <v>1.7999999999999999E-2</v>
@@ -4238,7 +4238,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B14" t="s">
         <v>367</v>
@@ -4247,10 +4247,10 @@
         <v>482</v>
       </c>
       <c r="D14" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E14" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="F14" t="s">
         <v>387</v>
@@ -4270,7 +4270,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="B15" t="s">
         <v>367</v>
@@ -4279,10 +4279,10 @@
         <v>482</v>
       </c>
       <c r="D15" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="E15" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F15" t="s">
         <v>387</v>
@@ -4330,31 +4330,31 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>598</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>599</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>600</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>601</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" t="s">
         <v>602</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>603</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>604</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>605</v>
-      </c>
-      <c r="M1" t="s">
-        <v>606</v>
       </c>
       <c r="N1" t="s">
         <v>361</v>
@@ -4362,7 +4362,7 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B2" t="s">
         <v>363</v>
@@ -4371,10 +4371,10 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="E2" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="F2">
         <v>1.75833333333333</v>
@@ -4406,7 +4406,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="B3" t="s">
         <v>363</v>
@@ -4415,7 +4415,7 @@
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="E3" t="s">
         <v>486</v>
@@ -4450,7 +4450,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B4" t="s">
         <v>363</v>
@@ -4459,7 +4459,7 @@
         <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="E4" t="s">
         <v>487</v>
@@ -4494,7 +4494,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B5" t="s">
         <v>363</v>
@@ -4503,10 +4503,10 @@
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E5" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="F5">
         <v>2.0633333333333299</v>
@@ -4538,7 +4538,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B6" t="s">
         <v>363</v>
@@ -4547,10 +4547,10 @@
         <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E6" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="F6">
         <v>2.165</v>
@@ -4582,7 +4582,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B7" t="s">
         <v>363</v>
@@ -4591,10 +4591,10 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="E7" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="F7">
         <v>2.2666666666666702</v>
@@ -4659,7 +4659,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>407</v>
@@ -4685,7 +4685,7 @@
         <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="E2" t="s">
         <v>395</v>
@@ -4714,10 +4714,10 @@
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E3" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -4743,7 +4743,7 @@
         <v>371</v>
       </c>
       <c r="D4" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E4" t="s">
         <v>71</v>
@@ -4772,10 +4772,10 @@
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E5" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -4792,7 +4792,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B6" t="s">
         <v>367</v>
@@ -4801,10 +4801,10 @@
         <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="E6" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -4821,7 +4821,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B7" t="s">
         <v>367</v>
@@ -4830,7 +4830,7 @@
         <v>371</v>
       </c>
       <c r="D7" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="E7" t="s">
         <v>458</v>
@@ -4850,7 +4850,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B8" t="s">
         <v>363</v>
@@ -4859,10 +4859,10 @@
         <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="E8" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -4879,7 +4879,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B9" t="s">
         <v>363</v>
@@ -4888,7 +4888,7 @@
         <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="E9" t="s">
         <v>486</v>
@@ -4908,7 +4908,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B10" t="s">
         <v>363</v>
@@ -4917,7 +4917,7 @@
         <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="E10" t="s">
         <v>487</v>
@@ -4937,7 +4937,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B11" t="s">
         <v>363</v>
@@ -4946,10 +4946,10 @@
         <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E11" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="F11">
         <v>1</v>
@@ -4966,7 +4966,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B12" t="s">
         <v>363</v>
@@ -4975,10 +4975,10 @@
         <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E12" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="F12">
         <v>1</v>
@@ -4995,7 +4995,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B13" t="s">
         <v>363</v>
@@ -5004,10 +5004,10 @@
         <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="E13" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="F13">
         <v>1</v>
@@ -5024,7 +5024,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B14" t="s">
         <v>367</v>
@@ -5033,10 +5033,10 @@
         <v>482</v>
       </c>
       <c r="D14" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E14" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="F14">
         <v>1</v>
@@ -5053,7 +5053,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B15" t="s">
         <v>367</v>
@@ -5062,10 +5062,10 @@
         <v>482</v>
       </c>
       <c r="D15" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="E15" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F15">
         <v>1</v>
@@ -5114,7 +5114,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>413</v>
@@ -5137,7 +5137,7 @@
         <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="E2" t="s">
         <v>395</v>
@@ -5163,10 +5163,10 @@
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E3" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="F3">
         <v>0.3</v>
@@ -5189,7 +5189,7 @@
         <v>371</v>
       </c>
       <c r="D4" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E4" t="s">
         <v>71</v>
@@ -5215,10 +5215,10 @@
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E5" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="F5">
         <v>1.7666666666666699</v>
@@ -5232,7 +5232,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B6" t="s">
         <v>367</v>
@@ -5241,10 +5241,10 @@
         <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="E6" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="F6">
         <v>2.06666666666667</v>
@@ -5258,7 +5258,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B7" t="s">
         <v>367</v>
@@ -5267,7 +5267,7 @@
         <v>371</v>
       </c>
       <c r="D7" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="E7" t="s">
         <v>458</v>
@@ -5284,7 +5284,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B8" t="s">
         <v>363</v>
@@ -5293,10 +5293,10 @@
         <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="E8" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="F8">
         <v>2.6666666666666701</v>
@@ -5310,7 +5310,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B9" t="s">
         <v>363</v>
@@ -5319,7 +5319,7 @@
         <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="E9" t="s">
         <v>486</v>
@@ -5336,7 +5336,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B10" t="s">
         <v>363</v>
@@ -5345,7 +5345,7 @@
         <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="E10" t="s">
         <v>487</v>
@@ -5362,7 +5362,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B11" t="s">
         <v>363</v>
@@ -5371,10 +5371,10 @@
         <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E11" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="F11">
         <v>3.56666666666667</v>
@@ -5388,7 +5388,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B12" t="s">
         <v>363</v>
@@ -5397,10 +5397,10 @@
         <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E12" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="F12">
         <v>3.8666666666666698</v>
@@ -5414,7 +5414,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B13" t="s">
         <v>363</v>
@@ -5423,10 +5423,10 @@
         <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="E13" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="F13">
         <v>4.1666666666666696</v>
@@ -5440,7 +5440,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B14" t="s">
         <v>367</v>
@@ -5449,10 +5449,10 @@
         <v>482</v>
       </c>
       <c r="D14" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E14" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="F14">
         <v>4.4666666666666703</v>
@@ -5466,7 +5466,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B15" t="s">
         <v>367</v>
@@ -5475,10 +5475,10 @@
         <v>482</v>
       </c>
       <c r="D15" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="E15" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F15">
         <v>4.7666666666666702</v>
@@ -5519,7 +5519,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>418</v>
@@ -5540,22 +5540,22 @@
         <v>423</v>
       </c>
       <c r="L1" s="8" t="s">
+        <v>633</v>
+      </c>
+      <c r="M1" s="9" t="s">
         <v>634</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="N1" s="9" t="s">
         <v>635</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="O1" s="10" t="s">
         <v>636</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="P1" s="8" t="s">
         <v>637</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="Q1" s="8" t="s">
         <v>638</v>
-      </c>
-      <c r="Q1" s="8" t="s">
-        <v>639</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>361</v>
@@ -5790,7 +5790,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>471</v>
@@ -5819,7 +5819,7 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="E2" t="s">
         <v>475</v>
@@ -5851,7 +5851,7 @@
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="E3" t="s">
         <v>365</v>
@@ -5883,7 +5883,7 @@
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="E4" t="s">
         <v>476</v>
@@ -5915,7 +5915,7 @@
         <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="E5" t="s">
         <v>476</v>
@@ -5938,7 +5938,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B6" t="s">
         <v>363</v>
@@ -5947,7 +5947,7 @@
         <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E6" t="s">
         <v>476</v>
@@ -5970,7 +5970,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B7" t="s">
         <v>477</v>
@@ -5979,7 +5979,7 @@
         <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E7" t="s">
         <v>476</v>
@@ -6009,7 +6009,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N30" sqref="N29:N30"/>
     </sheetView>
   </sheetViews>
@@ -6032,7 +6032,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>478</v>
@@ -6061,7 +6061,7 @@
         <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="E2" t="s">
         <v>395</v>
@@ -6093,10 +6093,10 @@
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E3" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="F3">
         <v>2</v>
@@ -6125,7 +6125,7 @@
         <v>371</v>
       </c>
       <c r="D4" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E4" t="s">
         <v>71</v>
@@ -6157,10 +6157,10 @@
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E5" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="F5">
         <v>2</v>
@@ -6180,7 +6180,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B6" t="s">
         <v>367</v>
@@ -6189,10 +6189,10 @@
         <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="E6" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -6212,7 +6212,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B7" t="s">
         <v>367</v>
@@ -6221,7 +6221,7 @@
         <v>371</v>
       </c>
       <c r="D7" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="E7" t="s">
         <v>458</v>
@@ -6244,7 +6244,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B8" t="s">
         <v>363</v>
@@ -6253,10 +6253,10 @@
         <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="E8" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -6276,7 +6276,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B9" t="s">
         <v>363</v>
@@ -6285,7 +6285,7 @@
         <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="E9" t="s">
         <v>486</v>
@@ -6308,7 +6308,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B10" t="s">
         <v>363</v>
@@ -6317,7 +6317,7 @@
         <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="E10" t="s">
         <v>487</v>
@@ -6340,7 +6340,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B11" t="s">
         <v>363</v>
@@ -6349,10 +6349,10 @@
         <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E11" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="F11">
         <v>1</v>
@@ -6372,7 +6372,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B12" t="s">
         <v>363</v>
@@ -6381,10 +6381,10 @@
         <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E12" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="F12">
         <v>2</v>
@@ -6404,7 +6404,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B13" t="s">
         <v>363</v>
@@ -6413,10 +6413,10 @@
         <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="E13" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="F13">
         <v>2</v>
@@ -6436,7 +6436,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B14" t="s">
         <v>367</v>
@@ -6445,10 +6445,10 @@
         <v>482</v>
       </c>
       <c r="D14" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E14" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="F14">
         <v>2</v>
@@ -6468,7 +6468,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B15" t="s">
         <v>367</v>
@@ -6477,10 +6477,10 @@
         <v>482</v>
       </c>
       <c r="D15" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="E15" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F15">
         <v>1</v>
@@ -6500,7 +6500,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B16" t="s">
         <v>363</v>
@@ -6509,10 +6509,10 @@
         <v>6</v>
       </c>
       <c r="D16" t="s">
+        <v>677</v>
+      </c>
+      <c r="E16" t="s">
         <v>678</v>
-      </c>
-      <c r="E16" t="s">
-        <v>679</v>
       </c>
       <c r="F16">
         <v>1</v>
@@ -6563,10 +6563,10 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>361</v>
@@ -6574,7 +6574,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B2" t="s">
         <v>363</v>
@@ -6583,21 +6583,21 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
+        <v>618</v>
+      </c>
+      <c r="E2" t="s">
         <v>619</v>
-      </c>
-      <c r="E2" t="s">
-        <v>620</v>
       </c>
       <c r="F2">
         <v>7.4</v>
       </c>
       <c r="G2" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B3" t="s">
         <v>363</v>
@@ -6606,21 +6606,21 @@
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="E3" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="F3">
         <v>11.7</v>
       </c>
       <c r="G3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="B4" t="s">
         <v>363</v>
@@ -6632,18 +6632,18 @@
         <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="F4">
         <v>33.1</v>
       </c>
       <c r="G4" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B5" t="s">
         <v>363</v>
@@ -6655,13 +6655,13 @@
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="F5">
         <v>33.1</v>
       </c>
       <c r="G5" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
   </sheetData>
@@ -6693,13 +6693,13 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>639</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>640</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>641</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>361</v>
@@ -6707,7 +6707,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="B2" t="s">
         <v>363</v>
@@ -6733,7 +6733,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="B3" t="s">
         <v>363</v>
@@ -6759,7 +6759,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="B4" t="s">
         <v>363</v>
@@ -6768,10 +6768,10 @@
         <v>7</v>
       </c>
       <c r="D4" t="s">
+        <v>666</v>
+      </c>
+      <c r="E4" t="s">
         <v>667</v>
-      </c>
-      <c r="E4" t="s">
-        <v>668</v>
       </c>
       <c r="F4">
         <v>0.6</v>
@@ -6785,7 +6785,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="B5" t="s">
         <v>363</v>
@@ -6797,7 +6797,7 @@
         <v>374</v>
       </c>
       <c r="E5" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="F5">
         <v>0.99</v>
@@ -6832,7 +6832,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="C1" t="s">
         <v>361</v>
@@ -6843,15 +6843,15 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="B2" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="B3" t="s">
         <v>41</v>
@@ -6859,7 +6859,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
@@ -6944,7 +6944,7 @@
         <v>359</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -6968,22 +6968,22 @@
         <v>433</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>607</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>608</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>609</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>610</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>611</v>
-      </c>
       <c r="O1" s="1" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -7030,10 +7030,10 @@
         <v>386</v>
       </c>
       <c r="O2" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="P2" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -7080,10 +7080,10 @@
         <v>388</v>
       </c>
       <c r="O3" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="P3" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -7130,10 +7130,10 @@
         <v>389</v>
       </c>
       <c r="O4" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="P4" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -7180,10 +7180,10 @@
         <v>391</v>
       </c>
       <c r="O5" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="P5" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -7230,10 +7230,10 @@
         <v>391</v>
       </c>
       <c r="O6" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="P6" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -7268,22 +7268,22 @@
         <v>443</v>
       </c>
       <c r="K7" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="L7" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="M7" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="N7" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="O7" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="P7" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -7330,10 +7330,10 @@
         <v>386</v>
       </c>
       <c r="O8" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="P8" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -7380,10 +7380,10 @@
         <v>388</v>
       </c>
       <c r="O9" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="P9" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -7430,10 +7430,10 @@
         <v>389</v>
       </c>
       <c r="O10" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="P10" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -7480,10 +7480,10 @@
         <v>391</v>
       </c>
       <c r="O11" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="P11" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -7530,10 +7530,10 @@
         <v>391</v>
       </c>
       <c r="O12" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="P12" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
@@ -7580,10 +7580,10 @@
         <v>389</v>
       </c>
       <c r="O13" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="P13" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
   </sheetData>
@@ -7609,7 +7609,7 @@
         <v>359</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -7627,21 +7627,21 @@
         <v>433</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>607</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>608</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>609</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>610</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>611</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B2" t="s">
         <v>482</v>
@@ -7650,7 +7650,7 @@
         <v>71</v>
       </c>
       <c r="D2" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="E2" t="s">
         <v>394</v>
@@ -7679,7 +7679,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B3" t="s">
         <v>482</v>
@@ -7688,16 +7688,16 @@
         <v>71</v>
       </c>
       <c r="D3" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="E3" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="F3" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="G3" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="H3" t="s">
         <v>436</v>
@@ -7724,8 +7724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7743,7 +7743,7 @@
         <v>359</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -7761,16 +7761,16 @@
         <v>430</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>607</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>608</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>609</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>610</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>611</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>433</v>
@@ -8153,7 +8153,7 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>489</v>
+        <v>679</v>
       </c>
       <c r="D11" t="s">
         <v>464</v>
@@ -8188,13 +8188,13 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B12" t="s">
         <v>371</v>
       </c>
       <c r="C12" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="D12" t="s">
         <v>372</v>
@@ -9894,7 +9894,7 @@
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="B55" t="s">
         <v>74</v>
@@ -9903,16 +9903,16 @@
         <v>2011</v>
       </c>
       <c r="D55" t="s">
+        <v>613</v>
+      </c>
+      <c r="E55" t="s">
         <v>614</v>
       </c>
-      <c r="E55" t="s">
+      <c r="F55" t="s">
         <v>615</v>
       </c>
-      <c r="F55" t="s">
-        <v>616</v>
-      </c>
       <c r="M55" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
   </sheetData>
@@ -9944,7 +9944,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>360</v>
@@ -9964,7 +9964,7 @@
         <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="E2" t="s">
         <v>395</v>
@@ -9987,10 +9987,10 @@
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E3" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="F3">
         <v>0.97599999999999998</v>
@@ -10010,7 +10010,7 @@
         <v>371</v>
       </c>
       <c r="D4" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E4" t="s">
         <v>71</v>
@@ -10033,10 +10033,10 @@
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E5" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="F5">
         <v>0.66</v>
@@ -10056,10 +10056,10 @@
         <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="E6" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="F6">
         <v>0.98</v>
@@ -10079,7 +10079,7 @@
         <v>371</v>
       </c>
       <c r="D7" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="E7" t="s">
         <v>458</v>
@@ -10102,10 +10102,10 @@
         <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="E8" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="F8">
         <v>0.89</v>
@@ -10125,7 +10125,7 @@
         <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="E9" t="s">
         <v>486</v>
@@ -10148,7 +10148,7 @@
         <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="E10" t="s">
         <v>487</v>
@@ -10171,10 +10171,10 @@
         <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E11" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="F11">
         <v>0.77</v>
@@ -10194,10 +10194,10 @@
         <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E12" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="F12">
         <v>0.77</v>
@@ -10208,7 +10208,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B13" t="s">
         <v>363</v>
@@ -10217,10 +10217,10 @@
         <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="E13" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="F13">
         <v>0.81</v>
@@ -10231,7 +10231,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B14" t="s">
         <v>367</v>
@@ -10240,10 +10240,10 @@
         <v>482</v>
       </c>
       <c r="D14" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E14" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="F14">
         <v>0.79213333333333302</v>
@@ -10254,7 +10254,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B15" t="s">
         <v>367</v>
@@ -10263,10 +10263,10 @@
         <v>482</v>
       </c>
       <c r="D15" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="E15" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F15">
         <v>0.78830303030303095</v>
@@ -10277,7 +10277,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B16" t="s">
         <v>367</v>
@@ -10286,10 +10286,10 @@
         <v>482</v>
       </c>
       <c r="D16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="E16" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F16">
         <v>0.78830303030303095</v>
@@ -10300,7 +10300,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="B17" t="s">
         <v>367</v>
@@ -10309,10 +10309,10 @@
         <v>482</v>
       </c>
       <c r="D17" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="E17" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F17">
         <v>0.78830303030303095</v>
@@ -10323,7 +10323,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B18" t="s">
         <v>367</v>
@@ -10332,10 +10332,10 @@
         <v>482</v>
       </c>
       <c r="D18" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="E18" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F18">
         <v>0.78830303030303095</v>
@@ -10373,19 +10373,19 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="F1" s="5" t="s">
+        <v>570</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>571</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>572</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>573</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>574</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>361</v>
@@ -10393,7 +10393,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B2" t="s">
         <v>363</v>
@@ -10402,10 +10402,10 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="E2" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="F2" s="7">
         <v>6</v>
@@ -10425,7 +10425,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="B3" t="s">
         <v>363</v>
@@ -10434,10 +10434,10 @@
         <v>6</v>
       </c>
       <c r="D3" t="s">
+        <v>628</v>
+      </c>
+      <c r="E3" t="s">
         <v>629</v>
-      </c>
-      <c r="E3" t="s">
-        <v>630</v>
       </c>
       <c r="F3" s="7">
         <v>7</v>
@@ -10457,7 +10457,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="B4" t="s">
         <v>363</v>
@@ -10469,7 +10469,7 @@
         <v>454</v>
       </c>
       <c r="E4" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="F4" s="7">
         <v>3</v>
@@ -10489,7 +10489,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="B5" t="s">
         <v>363</v>
@@ -10501,7 +10501,7 @@
         <v>449</v>
       </c>
       <c r="E5" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="F5" s="7">
         <v>4</v>
@@ -10548,7 +10548,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>382</v>
@@ -10577,7 +10577,7 @@
         <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="E2" t="s">
         <v>395</v>
@@ -10609,10 +10609,10 @@
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E3" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="F3" t="s">
         <v>387</v>
@@ -10641,7 +10641,7 @@
         <v>371</v>
       </c>
       <c r="D4" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E4" t="s">
         <v>71</v>
@@ -10673,13 +10673,13 @@
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E5" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="F5" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="G5">
         <v>7.0000000000000007E-2</v>
@@ -10696,7 +10696,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B6" t="s">
         <v>367</v>
@@ -10705,10 +10705,10 @@
         <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="E6" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="F6" t="s">
         <v>387</v>
@@ -10728,7 +10728,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B7" t="s">
         <v>367</v>
@@ -10737,7 +10737,7 @@
         <v>371</v>
       </c>
       <c r="D7" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="E7" t="s">
         <v>458</v>
@@ -10760,7 +10760,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B8" t="s">
         <v>363</v>
@@ -10769,10 +10769,10 @@
         <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="E8" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="F8" t="s">
         <v>390</v>
@@ -10792,7 +10792,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B9" t="s">
         <v>363</v>
@@ -10801,13 +10801,13 @@
         <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="E9" t="s">
         <v>486</v>
       </c>
       <c r="F9" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="G9">
         <v>4.2000000000000003E-2</v>
@@ -10824,7 +10824,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B10" t="s">
         <v>363</v>
@@ -10833,7 +10833,7 @@
         <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="E10" t="s">
         <v>487</v>
@@ -10856,7 +10856,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B11" t="s">
         <v>363</v>
@@ -10865,10 +10865,10 @@
         <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E11" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="F11" t="s">
         <v>387</v>
@@ -10888,7 +10888,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B12" t="s">
         <v>363</v>
@@ -10897,10 +10897,10 @@
         <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E12" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="F12" t="s">
         <v>390</v>
@@ -10920,7 +10920,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B13" t="s">
         <v>363</v>
@@ -10929,13 +10929,13 @@
         <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="E13" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="F13" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="G13">
         <v>1.7999999999999999E-2</v>
@@ -10952,7 +10952,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B14" t="s">
         <v>367</v>
@@ -10961,10 +10961,10 @@
         <v>482</v>
       </c>
       <c r="D14" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E14" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="F14" t="s">
         <v>387</v>
@@ -10984,7 +10984,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B15" t="s">
         <v>367</v>
@@ -10993,10 +10993,10 @@
         <v>482</v>
       </c>
       <c r="D15" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="E15" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F15" t="s">
         <v>387</v>

</xml_diff>